<commit_message>
1.vs增加binding protocol="http" bindingInformation="*:21021:192.168.5.169" / 2.修改图片保存地址避免发布覆盖；
</commit_message>
<xml_diff>
--- a/src/Capinfo.Web.Host/wwwroot/工作周报_吴海龙.xlsx
+++ b/src/Capinfo.Web.Host/wwwroot/工作周报_吴海龙.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>工作周报</t>
   </si>
@@ -22,7 +22,7 @@
     <t>姓名</t>
   </si>
   <si>
-    <t>海龙</t>
+    <t>穆琨</t>
   </si>
   <si>
     <t>岗位</t>
@@ -34,7 +34,7 @@
     <t>日期：</t>
   </si>
   <si>
-    <t>2020-02-23 - 2020-03-01</t>
+    <t>2020-03-02 - 2020-03-08</t>
   </si>
   <si>
     <t>序号</t>
@@ -70,9 +70,6 @@
     <t>已完成</t>
   </si>
   <si>
-    <t>2020/2/24 0:00:00 88 8888</t>
-  </si>
-  <si>
     <t>日常维护——权限</t>
   </si>
   <si>
@@ -80,12 +77,6 @@
   </si>
   <si>
     <t>日常维护——咨询</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/2/29 16:00:00 2223333 2223333222333322233332223333
-2020/2/29 16:00:00 2223333 2223333222333322233332223333
-2020/3/1 16:20:00 6 666666
-2020/3/1 16:22:43 6 666666</t>
   </si>
   <si>
     <t>日常维护——开发工作</t>
@@ -1394,9 +1385,7 @@
       <c r="E4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="64" t="s">
-        <v>18</v>
-      </c>
+      <c r="F4" s="64"/>
       <c r="G4" s="65"/>
       <c r="H4" s="65"/>
       <c r="I4" s="65"/>
@@ -1408,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="61"/>
       <c r="D5" s="62"/>
@@ -1427,7 +1416,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="67"/>
       <c r="D6" s="68"/>
@@ -1446,16 +1435,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="70"/>
       <c r="D7" s="70"/>
       <c r="E7" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="64" t="s">
-        <v>22</v>
-      </c>
+      <c r="F7" s="64"/>
       <c r="G7" s="65"/>
       <c r="H7" s="65"/>
       <c r="I7" s="65"/>
@@ -1467,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="72"/>
       <c r="D8" s="73"/>
@@ -1486,12 +1473,12 @@
         <v>6</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="70"/>
       <c r="D9" s="70"/>
       <c r="E9" s="63" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="74"/>
       <c r="G9" s="65"/>

</xml_diff>